<commit_message>
test now all working except for the interp test and the xlsx file now expands to the individual inputs
</commit_message>
<xml_diff>
--- a/__test__/resources/resourcesData.xlsx
+++ b/__test__/resources/resourcesData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CODE\PLG\__test__\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627F6195-439B-4361-B465-F9D6E880FA49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D981A723-1439-4289-871C-B4796B980FDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="1530" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="basicGeom" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,12 +252,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -665,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +717,7 @@
         <v>0.89986292564075221</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C13" si="1">H5*SIN(RADIANS(G5))</f>
@@ -746,7 +740,7 @@
         <v>0.79221445499325638</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -769,7 +763,7 @@
         <v>0.684703320513664</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -792,7 +786,7 @@
         <v>0.57063390977709216</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -815,7 +809,7 @@
         <v>0.64902869819675124</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -838,7 +832,7 @@
         <v>0.70635807428714159</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -861,7 +855,7 @@
         <v>0.76324328654078333</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -884,7 +878,7 @@
         <v>3.489949670250108E-2</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -907,7 +901,7 @@
         <v>6.7383165019974101E-17</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -1045,7 +1039,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1053,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF165B81-2137-4288-9910-674D48D9CE9E}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>